<commit_message>
Defined model for pm2_batch
Defined model metrics for pm2_batch
</commit_message>
<xml_diff>
--- a/exposan/pm2/data/stoichio.xlsx
+++ b/exposan/pm2/data/stoichio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Downloads\EXPOsan\exposan\pm2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FE3D8B-A353-43CA-BA36-41064A197DF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA515CB3-A36E-476D-BC64-067F3ED2387D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,7 +171,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -249,7 +249,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -561,7 +561,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="M3" sqref="M3:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2222,59 +2222,59 @@
         <v>46</v>
       </c>
       <c r="B33" s="2">
-        <f>SUMPRODUCT(B2:B31,$P$2:$P$31)</f>
+        <f t="shared" ref="B33:O33" si="0">SUMPRODUCT(B2:B31,$P$2:$P$31)</f>
         <v>0.185786304971432</v>
       </c>
       <c r="C33" s="2">
-        <f>SUMPRODUCT(C2:C31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>112.38901818557167</v>
       </c>
       <c r="D33" s="2">
-        <f>SUMPRODUCT(D2:D31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-129.14122771055546</v>
       </c>
       <c r="E33" s="2">
-        <f>SUMPRODUCT(E2:E31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-218.44796291841902</v>
       </c>
       <c r="F33" s="2">
-        <f>SUMPRODUCT(F2:F31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>254.81393428405946</v>
       </c>
       <c r="G33" s="2">
-        <f>SUMPRODUCT(G2:G31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-4.0904629719543379</v>
       </c>
       <c r="H33" s="2">
-        <f>SUMPRODUCT(H2:H31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-3.1038739458993101</v>
       </c>
       <c r="I33" s="2">
-        <f>SUMPRODUCT(I2:I31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-241.29145894755658</v>
       </c>
       <c r="J33" s="2">
-        <f>SUMPRODUCT(J2:J31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-7.3149292435336575</v>
       </c>
       <c r="K33" s="2">
-        <f>SUMPRODUCT(K2:K31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-0.24141680671728238</v>
       </c>
       <c r="L33" s="2">
-        <f>SUMPRODUCT(L2:L31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-0.43806043864819499</v>
       </c>
       <c r="M33" s="2">
-        <f>SUMPRODUCT(M2:M31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-1.6176533419747932</v>
       </c>
       <c r="N33" s="2">
-        <f>SUMPRODUCT(N2:N31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>-1.3877653313765161</v>
       </c>
       <c r="O33" s="2">
-        <f>SUMPRODUCT(O2:O31,$P$2:$P$31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>